<commit_message>
FI_T col header redeclared case: ACT_EFF of IDM1ETOT in REG1 is 1.5
</commit_message>
<xml_diff>
--- a/VT_REG1_IND_V12.xlsx
+++ b/VT_REG1_IND_V12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\Model_Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D68DB0D-BEE9-4E7C-8204-A3BF2700AE8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D314F7-A4D6-43EF-A0EE-91A31AF64D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="1335" windowWidth="18135" windowHeight="11025" tabRatio="901" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" tabRatio="901" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EB1" sheetId="133" r:id="rId1"/>
@@ -820,7 +820,7 @@
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -934,7 +934,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="R3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -960,7 +960,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="S3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1033,7 +1033,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="T3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1086,7 +1086,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="U3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1119,7 +1119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R9" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
+    <comment ref="S9" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1212,7 +1212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+    <comment ref="T9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1237,7 +1237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T9" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+    <comment ref="U9" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1300,7 +1300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L10" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
+    <comment ref="M10" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1548,7 +1548,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="163">
   <si>
     <t>CommName</t>
   </si>
@@ -3264,13 +3264,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>123824</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>3811972</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -3660,7 +3660,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="IEA Data"/>
@@ -3795,7 +3795,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="EnergyBalance"/>
@@ -4595,24 +4595,24 @@
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="21" width="10.85546875" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="21" width="10.86328125" customWidth="1"/>
+    <col min="22" max="22" width="7.265625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.265625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="45" width="10.85546875" customWidth="1"/>
+    <col min="29" max="29" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="45" width="10.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" s="5" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="X1" s="26" t="s">
         <v>94</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" ht="15.75" x14ac:dyDescent="0.5">
       <c r="C2" s="6"/>
       <c r="D2" s="47" t="s">
         <v>44</v>
@@ -4742,7 +4742,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" ht="39.4" x14ac:dyDescent="0.4">
       <c r="C3" s="82" t="s">
         <v>119</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B4" s="45"/>
       <c r="C4" s="98" t="s">
         <v>59</v>
@@ -4899,7 +4899,7 @@
       <c r="AR4" s="6"/>
       <c r="AS4" s="6"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A5" s="5"/>
       <c r="B5" s="49" t="s">
         <v>60</v>
@@ -5035,7 +5035,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A6" s="5"/>
       <c r="B6" s="49" t="s">
         <v>62</v>
@@ -5171,7 +5171,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="B7" s="49" t="s">
         <v>64</v>
@@ -5308,7 +5308,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A8" s="5"/>
       <c r="B8" s="49" t="s">
         <v>66</v>
@@ -5444,7 +5444,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
       <c r="B9" s="49" t="s">
         <v>68</v>
@@ -5580,7 +5580,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
       <c r="B10" s="49" t="s">
         <v>70</v>
@@ -5716,7 +5716,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A11" s="5"/>
       <c r="B11" s="49" t="s">
         <v>87</v>
@@ -5852,7 +5852,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A12" s="5"/>
       <c r="B12" s="49" t="s">
         <v>88</v>
@@ -5988,7 +5988,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="13" spans="1:45" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="5"/>
       <c r="B13" s="97" t="s">
         <v>90</v>
@@ -6080,7 +6080,7 @@
       <c r="AR13" s="69"/>
       <c r="AS13" s="70"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="D14" s="10"/>
       <c r="F14" s="10"/>
@@ -6092,7 +6092,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="D15" s="10"/>
       <c r="F15" s="10"/>
@@ -6104,7 +6104,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:45" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="5"/>
       <c r="C16" s="52" t="s">
         <v>141</v>
@@ -6120,7 +6120,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="D17" s="10"/>
       <c r="F17" s="10"/>
@@ -6132,12 +6132,12 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="C18" s="27"/>
       <c r="D18" s="28"/>
     </row>
-    <row r="19" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" ht="39.4" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
       <c r="B19" s="29" t="s">
         <v>102</v>
@@ -6203,7 +6203,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="5"/>
       <c r="B20" s="111" t="s">
         <v>64</v>
@@ -6237,15 +6237,15 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="V21" s="7"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="V22" s="7"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A23" s="5"/>
       <c r="C23" s="64" t="s">
         <v>107</v>
@@ -6258,7 +6258,7 @@
       </c>
       <c r="V23" s="7"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A24" s="5"/>
       <c r="B24" s="26" t="s">
         <v>117</v>
@@ -6274,7 +6274,7 @@
       </c>
       <c r="V24" s="7"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A25" s="5"/>
       <c r="B25" s="49" t="s">
         <v>64</v>
@@ -6300,19 +6300,19 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="4" width="6.85546875" customWidth="1"/>
+    <col min="1" max="1" width="1.86328125" customWidth="1"/>
+    <col min="2" max="2" width="7.73046875" customWidth="1"/>
+    <col min="3" max="4" width="6.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="B2" s="89" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="E4" s="114"/>
       <c r="F4" s="114"/>
       <c r="G4" s="114"/>
@@ -6320,7 +6320,7 @@
       <c r="I4" s="114"/>
       <c r="J4" s="114"/>
     </row>
-    <row r="5" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E5" s="90" t="s">
         <v>153</v>
       </c>
@@ -6341,33 +6341,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.3984375" customWidth="1"/>
+    <col min="11" max="11" width="7.1328125" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="63" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" customWidth="1"/>
+    <col min="14" max="14" width="6.1328125" customWidth="1"/>
+    <col min="15" max="15" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B1" s="11" t="s">
         <v>75</v>
       </c>
@@ -6388,7 +6388,7 @@
       </c>
       <c r="H1" s="38"/>
     </row>
-    <row r="2" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B2" s="13" t="str">
         <f>'EB1'!B7</f>
         <v>IND</v>
@@ -6424,7 +6424,7 @@
       <c r="Q2" s="137"/>
       <c r="R2" s="137"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="J3" s="138" t="s">
         <v>7</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:18" s="5" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" s="5" customFormat="1" ht="22.15" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -6487,7 +6487,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -6516,7 +6516,7 @@
       <c r="Q5" s="141"/>
       <c r="R5" s="141"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -6543,7 +6543,7 @@
       <c r="Q6" s="141"/>
       <c r="R6" s="141"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -6570,7 +6570,7 @@
       <c r="Q7" s="141"/>
       <c r="R7" s="141"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -6597,7 +6597,7 @@
       <c r="Q8" s="141"/>
       <c r="R8" s="141"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -6628,7 +6628,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -6646,7 +6646,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -6657,7 +6657,7 @@
       <c r="L11" s="31"/>
       <c r="M11" s="33"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -6675,7 +6675,7 @@
       <c r="Q12" s="143"/>
       <c r="R12" s="143"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B13" s="21" t="s">
         <v>1</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:18" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="19" t="s">
         <v>39</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="18" t="s">
         <v>92</v>
       </c>
@@ -6802,7 +6802,7 @@
       <c r="Q15" s="144"/>
       <c r="R15" s="144"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B16" t="str">
         <f>L16</f>
         <v>FTE-INDCOA</v>
@@ -6847,7 +6847,7 @@
       <c r="Q16" s="141"/>
       <c r="R16" s="141"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B17" t="str">
         <f>L17</f>
         <v>FTE-INDGAS</v>
@@ -6890,7 +6890,7 @@
       <c r="Q17" s="141"/>
       <c r="R17" s="141"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f>L18</f>
         <v>FTE-INDOIL</v>
@@ -6936,7 +6936,7 @@
       <c r="Q18" s="141"/>
       <c r="R18" s="141"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C19" t="str">
         <f>'EB1'!H$2</f>
         <v>KER</v>
@@ -6970,7 +6970,7 @@
       <c r="Q19" s="141"/>
       <c r="R19" s="141"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C20" t="str">
         <f>'EB1'!I$2</f>
         <v>LPG</v>
@@ -7006,7 +7006,7 @@
       <c r="Q20" s="141"/>
       <c r="R20" s="141"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C21" t="str">
         <f>'EB1'!J$2</f>
         <v>GSL</v>
@@ -7028,7 +7028,7 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C22" t="str">
         <f>'EB1'!K$2</f>
         <v>NAP</v>
@@ -7050,7 +7050,7 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C23" t="str">
         <f>'EB1'!L$2</f>
         <v>HFO</v>
@@ -7072,7 +7072,7 @@
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
       <c r="C24" t="str">
         <f>'EB1'!M$2</f>
         <v>OPP</v>
@@ -7094,7 +7094,7 @@
       <c r="Q24" s="36"/>
       <c r="R24" s="5"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B25" t="str">
         <f>L19</f>
         <v>FTE-INDBIO</v>
@@ -7116,7 +7116,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B26" t="str">
         <f>L20</f>
         <v>FTE-INDELC</v>
@@ -7138,7 +7138,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -7147,7 +7147,7 @@
       <c r="G27" s="88"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B28" s="116"/>
       <c r="C28" s="5"/>
       <c r="D28" s="116"/>
@@ -7156,7 +7156,7 @@
       <c r="G28" s="88"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B29" s="116"/>
       <c r="C29" s="5"/>
       <c r="D29" s="116"/>
@@ -7165,7 +7165,7 @@
       <c r="G29" s="88"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B30" s="116"/>
       <c r="C30" s="5"/>
       <c r="D30" s="116"/>
@@ -7174,13 +7174,13 @@
       <c r="G30" s="88"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="50"/>
       <c r="C34" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="83"/>
       <c r="C35" s="1" t="s">
         <v>144</v>
@@ -7196,37 +7196,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:T27"/>
+  <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="2" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" customWidth="1"/>
+    <col min="10" max="10" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.1328125" customWidth="1"/>
+    <col min="12" max="12" width="2" customWidth="1"/>
+    <col min="13" max="13" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1328125" customWidth="1"/>
+    <col min="15" max="15" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="63.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.73046875" customWidth="1"/>
+    <col min="18" max="18" width="11.73046875" customWidth="1"/>
+    <col min="19" max="19" width="13.3984375" customWidth="1"/>
+    <col min="20" max="20" width="13.86328125" customWidth="1"/>
+    <col min="21" max="21" width="8.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B1" s="11" t="s">
         <v>75</v>
       </c>
@@ -7243,11 +7244,11 @@
         <v>80</v>
       </c>
       <c r="G1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B2" s="13" t="str">
         <f>'EB1'!B7</f>
         <v>IND</v>
@@ -7269,51 +7270,51 @@
         <v>M€2005</v>
       </c>
       <c r="G2" s="13"/>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="136" t="s">
+      <c r="M2" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="136"/>
-      <c r="N2" s="137"/>
+      <c r="N2" s="136"/>
       <c r="O2" s="137"/>
       <c r="P2" s="137"/>
       <c r="Q2" s="137"/>
       <c r="R2" s="137"/>
       <c r="S2" s="137"/>
       <c r="T2" s="137"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="L3" s="138" t="s">
+      <c r="U2" s="137"/>
+    </row>
+    <row r="3" spans="2:21" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="M3" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="139" t="s">
+      <c r="N3" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="138" t="s">
-        <v>0</v>
-      </c>
       <c r="O3" s="138" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="138" t="s">
+      <c r="Q3" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="138" t="s">
+      <c r="R3" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="138" t="s">
+      <c r="S3" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="138" t="s">
+      <c r="T3" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="138" t="s">
+      <c r="U3" s="138" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:20" s="5" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:21" s="5" customFormat="1" ht="22.15" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -7321,35 +7322,36 @@
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
-      <c r="L4" s="140" t="s">
+      <c r="I4" s="12"/>
+      <c r="M4" s="140" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="140" t="s">
+      <c r="N4" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="140" t="s">
+      <c r="O4" s="140" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="140" t="s">
+      <c r="P4" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="140" t="s">
+      <c r="Q4" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="140" t="s">
+      <c r="R4" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="140" t="s">
+      <c r="S4" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="140" t="s">
+      <c r="T4" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="140" t="s">
+      <c r="U4" s="140" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:20" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -7357,55 +7359,56 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
-      <c r="L5" s="145" t="s">
+      <c r="I5" s="12"/>
+      <c r="M5" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="M5" s="141"/>
-      <c r="N5" s="145" t="str">
-        <f>LEFT($L$5,1)&amp;LEFT(B2,1)&amp;'EB1'!$C$20</f>
+      <c r="N5" s="141"/>
+      <c r="O5" s="145" t="str">
+        <f>LEFT($M$5,1)&amp;LEFT(B2,1)&amp;'EB1'!$C$20</f>
         <v>DIDM1</v>
       </c>
-      <c r="O5" s="145" t="str">
+      <c r="P5" s="145" t="str">
         <f>LEFT($D$2,6)&amp;" "&amp;$C$2&amp; " Sector - "&amp;'EB1'!$X$20</f>
         <v>Demand Industry Sector - Demand 1</v>
       </c>
-      <c r="P5" s="145" t="str">
+      <c r="Q5" s="145" t="str">
         <f>$E$2</f>
         <v>PJ</v>
       </c>
-      <c r="Q5" s="145"/>
       <c r="R5" s="145"/>
       <c r="S5" s="145"/>
       <c r="T5" s="145"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="L6" s="143" t="s">
+      <c r="U5" s="145"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="M6" s="143" t="s">
         <v>106</v>
       </c>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143" t="str">
+      <c r="N6" s="143"/>
+      <c r="O6" s="143" t="str">
         <f>$B$2&amp;'EB1'!$C$23</f>
         <v>INDCO2</v>
       </c>
-      <c r="O6" s="143" t="str">
+      <c r="P6" s="143" t="str">
         <f>$C$2&amp;" "&amp;'EB1'!$C$24</f>
         <v>Industry Carbon dioxide</v>
       </c>
-      <c r="P6" s="143" t="str">
+      <c r="Q6" s="143" t="str">
         <f>'EB1'!$AA$2</f>
         <v>kt</v>
       </c>
-      <c r="Q6" s="143"/>
       <c r="R6" s="143"/>
       <c r="S6" s="143"/>
       <c r="T6" s="143"/>
-    </row>
-    <row r="7" spans="2:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="U6" s="143"/>
+    </row>
+    <row r="7" spans="2:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="G7" s="128" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
@@ -7414,21 +7417,21 @@
       <c r="G8" s="129">
         <v>0.2</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="17"/>
-      <c r="L8" s="136" t="s">
+      <c r="J8" s="4"/>
+      <c r="K8" s="17"/>
+      <c r="M8" s="136" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="136"/>
-      <c r="N8" s="143"/>
+      <c r="N8" s="136"/>
       <c r="O8" s="143"/>
       <c r="P8" s="143"/>
       <c r="Q8" s="143"/>
       <c r="R8" s="143"/>
       <c r="S8" s="143"/>
       <c r="T8" s="143"/>
-    </row>
-    <row r="9" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="U8" s="143"/>
+    </row>
+    <row r="9" spans="2:21" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B9" s="21" t="s">
         <v>1</v>
       </c>
@@ -7451,40 +7454,43 @@
         <v>86</v>
       </c>
       <c r="I9" s="91" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="91" t="s">
+      <c r="K9" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="L9" s="138" t="s">
+      <c r="M9" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="139" t="s">
+      <c r="N9" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="N9" s="138" t="s">
+      <c r="O9" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="138" t="s">
+      <c r="P9" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="P9" s="138" t="s">
+      <c r="Q9" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="Q9" s="138" t="s">
+      <c r="R9" s="138" t="s">
         <v>17</v>
       </c>
-      <c r="R9" s="138" t="s">
+      <c r="S9" s="138" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="138" t="s">
+      <c r="T9" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="138" t="s">
+      <c r="U9" s="138" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:20" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="19" t="s">
         <v>39</v>
       </c>
@@ -7506,41 +7512,42 @@
       <c r="H10" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="104" t="s">
+      <c r="I10" s="19"/>
+      <c r="J10" s="104" t="s">
         <v>99</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="K10" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="L10" s="140" t="s">
+      <c r="M10" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="M10" s="140" t="s">
+      <c r="N10" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="N10" s="140" t="s">
+      <c r="O10" s="140" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="140" t="s">
+      <c r="P10" s="140" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="140" t="s">
+      <c r="Q10" s="140" t="s">
         <v>23</v>
       </c>
-      <c r="Q10" s="140" t="s">
+      <c r="R10" s="140" t="s">
         <v>24</v>
       </c>
-      <c r="R10" s="140" t="s">
+      <c r="S10" s="140" t="s">
         <v>43</v>
       </c>
-      <c r="S10" s="140" t="s">
+      <c r="T10" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="T10" s="140" t="s">
+      <c r="U10" s="140" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="18" t="s">
         <v>92</v>
       </c>
@@ -7554,13 +7561,13 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="93"/>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="93"/>
+      <c r="K11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="L11" s="140" t="s">
+      <c r="M11" s="140" t="s">
         <v>83</v>
       </c>
-      <c r="M11" s="140"/>
       <c r="N11" s="140"/>
       <c r="O11" s="140"/>
       <c r="P11" s="140"/>
@@ -7568,10 +7575,11 @@
       <c r="R11" s="140"/>
       <c r="S11" s="140"/>
       <c r="T11" s="140"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U11" s="140"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B12" t="str">
-        <f>N12</f>
+        <f>O12</f>
         <v>IDM1ETOT</v>
       </c>
       <c r="C12" t="str">
@@ -7579,7 +7587,7 @@
         <v>INDCOA</v>
       </c>
       <c r="D12" t="str">
-        <f>$N$5</f>
+        <f>$O$5</f>
         <v>DIDM1</v>
       </c>
       <c r="E12" s="118"/>
@@ -7595,36 +7603,39 @@
         <v>1</v>
       </c>
       <c r="I12" s="87">
+        <v>1.5</v>
+      </c>
+      <c r="J12" s="87">
         <v>0.95</v>
       </c>
-      <c r="J12" s="50">
+      <c r="K12" s="50">
         <v>30</v>
       </c>
-      <c r="L12" s="145" t="s">
+      <c r="M12" s="145" t="s">
         <v>97</v>
       </c>
-      <c r="M12" s="141"/>
-      <c r="N12" s="141" t="str">
-        <f>LEFT($B$2)&amp;'EB1'!$C$20&amp;$I$2&amp;'EB1'!V2</f>
+      <c r="N12" s="141"/>
+      <c r="O12" s="141" t="str">
+        <f>LEFT($B$2)&amp;'EB1'!$C$20&amp;$J$2&amp;'EB1'!V2</f>
         <v>IDM1ETOT</v>
       </c>
-      <c r="O12" s="146" t="str">
-        <f>$D$2&amp;" "&amp;$C$2&amp; " Sector - "&amp;""&amp;$I$1&amp;" "&amp;'EB1'!$X$20&amp;" - "&amp;'EB1'!$V$3</f>
+      <c r="P12" s="146" t="str">
+        <f>$D$2&amp;" "&amp;$C$2&amp; " Sector - "&amp;""&amp;$J$1&amp;" "&amp;'EB1'!$X$20&amp;" - "&amp;'EB1'!$V$3</f>
         <v>Demand Technologies Industry Sector - Existing Demand 1 - Total</v>
       </c>
-      <c r="P12" s="141" t="str">
+      <c r="Q12" s="141" t="str">
         <f>$E$2</f>
         <v>PJ</v>
       </c>
-      <c r="Q12" s="141" t="str">
+      <c r="R12" s="141" t="str">
         <f>$E$2&amp;"a"</f>
         <v>PJa</v>
       </c>
-      <c r="R12" s="141"/>
       <c r="S12" s="141"/>
       <c r="T12" s="141"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U12" s="141"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C13" t="str">
         <f>Sector_Fuels!L6</f>
         <v>INDGAS</v>
@@ -7639,17 +7650,18 @@
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
-      <c r="L13" s="5"/>
+      <c r="J13" s="20"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="25"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U13" s="5"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
       <c r="C14" t="str">
         <f>Sector_Fuels!L7</f>
@@ -7667,18 +7679,19 @@
       </c>
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
-      <c r="J14" s="7"/>
-      <c r="L14" s="5"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="7"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="25"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U14" s="5"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" t="str">
         <f>Sector_Fuels!L8</f>
@@ -7695,18 +7708,19 @@
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
-      <c r="J15" s="7"/>
-      <c r="L15" s="5"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="7"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="25"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C16" t="str">
         <f>Sector_Fuels!L9</f>
         <v>INDELC</v>
@@ -7719,7 +7733,6 @@
         <f>IF(F16=0,20%,F16*(1+$G$8))</f>
         <v>0.37162920096559471</v>
       </c>
-      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -7728,15 +7741,16 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U16" s="5"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="119"/>
       <c r="G17" s="119"/>
       <c r="H17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="I17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -7745,11 +7759,11 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U17" s="5"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="F18" s="120"/>
       <c r="G18" s="120"/>
-      <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -7758,11 +7772,11 @@
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U18" s="5"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="F19" s="120"/>
       <c r="G19" s="120"/>
-      <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
@@ -7771,11 +7785,12 @@
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U19" s="5"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="H20" s="10"/>
-      <c r="I20" s="126"/>
-      <c r="L20" s="5"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="126"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
@@ -7784,10 +7799,10 @@
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="I21" s="126"/>
-      <c r="L21" s="5"/>
+      <c r="U20" s="5"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="J21" s="126"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -7796,37 +7811,38 @@
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B22" s="50"/>
       <c r="C22" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I22" s="126"/>
-    </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="J22" s="126"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B23" s="83"/>
       <c r="C23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I23" s="126"/>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="I24" s="126"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="J23" s="126"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="J24" s="126"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D27" s="5"/>
       <c r="E27" s="118"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7843,24 +7859,24 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.265625" customWidth="1"/>
+    <col min="8" max="8" width="15.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1328125" customWidth="1"/>
+    <col min="11" max="11" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.59765625" customWidth="1"/>
     <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B1" s="11" t="s">
         <v>75</v>
       </c>
@@ -7877,7 +7893,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B2" s="13" t="s">
         <v>85</v>
       </c>
@@ -7892,14 +7908,14 @@
         <v>M€2005</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:15" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>82</v>
       </c>
@@ -7913,7 +7929,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15" ht="20.65" x14ac:dyDescent="0.35">
       <c r="B7" s="19" t="s">
         <v>83</v>
       </c>
@@ -7927,7 +7943,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="18" t="s">
         <v>92</v>
       </c>
@@ -7942,12 +7958,12 @@
       <c r="N8" s="36"/>
       <c r="O8" s="36"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="7" t="str">
-        <f>DemTechs_IND!$N$5</f>
+        <f>DemTechs_IND!$O$5</f>
         <v>DIDM1</v>
       </c>
       <c r="D9" s="27" t="s">
@@ -7962,13 +7978,13 @@
       <c r="N9" s="36"/>
       <c r="O9" s="36"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="L10" s="150"/>
       <c r="M10" s="36"/>
       <c r="N10" s="36"/>
       <c r="O10" s="36"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="36"/>
       <c r="C11" s="36"/>
       <c r="D11" s="121"/>
@@ -7978,7 +7994,7 @@
       <c r="N11" s="36"/>
       <c r="O11" s="36"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B12" s="36"/>
       <c r="C12" s="36"/>
       <c r="D12" s="121"/>
@@ -7987,7 +8003,7 @@
       <c r="N12" s="124"/>
       <c r="O12" s="36"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
       <c r="D13" s="121"/>
@@ -7996,7 +8012,7 @@
       <c r="N13" s="124"/>
       <c r="O13" s="36"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
       <c r="D14" s="121"/>
@@ -8005,7 +8021,7 @@
       <c r="N14" s="36"/>
       <c r="O14" s="36"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
       <c r="D15" s="121"/>
@@ -8014,7 +8030,7 @@
       <c r="N15" s="36"/>
       <c r="O15" s="36"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B16" s="36"/>
       <c r="C16" s="36"/>
       <c r="D16" s="121"/>
@@ -8023,7 +8039,7 @@
       <c r="N16" s="36"/>
       <c r="O16" s="36"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" s="36"/>
       <c r="C17" s="36"/>
       <c r="D17" s="121"/>
@@ -8032,7 +8048,7 @@
       <c r="N17" s="36"/>
       <c r="O17" s="36"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
       <c r="D18" s="121"/>
@@ -8041,7 +8057,7 @@
       <c r="N18" s="124"/>
       <c r="O18" s="36"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
       <c r="D19" s="121"/>
@@ -8051,7 +8067,7 @@
       <c r="N19" s="124"/>
       <c r="O19" s="36"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
       <c r="D20" s="121"/>
@@ -8061,14 +8077,14 @@
       <c r="N20" s="36"/>
       <c r="O20" s="36"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K21" s="149"/>
       <c r="L21" s="36"/>
       <c r="M21" s="36"/>
       <c r="N21" s="36"/>
       <c r="O21" s="36"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
       <c r="J22" s="147"/>
       <c r="K22" s="149"/>
       <c r="L22" s="36"/>
@@ -8076,7 +8092,7 @@
       <c r="N22" s="36"/>
       <c r="O22" s="36"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
       <c r="E23" s="34"/>
       <c r="K23" s="149"/>
       <c r="L23" s="36"/>
@@ -8084,7 +8100,7 @@
       <c r="N23" s="124"/>
       <c r="O23" s="36"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
       <c r="E24" s="10"/>
       <c r="K24" s="149"/>
       <c r="L24" s="36"/>
@@ -8092,32 +8108,32 @@
       <c r="N24" s="36"/>
       <c r="O24" s="36"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K25" s="149"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
       <c r="E26" s="10"/>
       <c r="K26" s="149"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K27" s="149"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K28" s="149"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K29" s="149"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
       <c r="K30" s="149"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B32" s="50"/>
       <c r="C32" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="83"/>
       <c r="C33" s="1" t="s">
         <v>144</v>
@@ -8138,12 +8154,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="41" t="s">
         <v>150</v>
       </c>
@@ -8155,7 +8171,7 @@
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
     </row>
-    <row r="4" spans="2:9" s="5" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" s="5" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
@@ -8163,7 +8179,7 @@
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
     </row>
-    <row r="5" spans="2:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="17.25" x14ac:dyDescent="0.45">
       <c r="B5" s="39" t="s">
         <v>135</v>
       </c>
@@ -8171,7 +8187,7 @@
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
     </row>
-    <row r="6" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="44" t="s">
         <v>0</v>
       </c>
@@ -8191,7 +8207,7 @@
       <c r="G6" s="43"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="18" t="s">
         <v>92</v>
       </c>
@@ -8208,9 +8224,9 @@
       <c r="G7" s="123"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B8" s="43" t="str">
-        <f>DemTechs_IND!N6</f>
+        <f>DemTechs_IND!O6</f>
         <v>INDCO2</v>
       </c>
       <c r="C8" s="87">
@@ -8226,17 +8242,17 @@
       <c r="G8" s="124"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="F9" s="36"/>
       <c r="G9" s="36"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="50"/>
       <c r="C23" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="83"/>
       <c r="C24" s="1" t="s">
         <v>144</v>

</xml_diff>